<commit_message>
added tagging feature to swirl -- tell user what topics they struggled with
</commit_message>
<xml_diff>
--- a/inst/Data_Analysis_Modules/Module1.xlsx
+++ b/inst/Data_Analysis_Modules/Module1.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A:$J</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A:$K</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="76">
   <si>
     <t>Choices</t>
   </si>
@@ -227,6 +227,30 @@
   </si>
   <si>
     <t>Would you like to watch a brief video on mean, median, and mode?</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>central tendency</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>sample vs. population</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>mode</t>
   </si>
 </sst>
 </file>
@@ -279,7 +303,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -302,12 +326,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -327,6 +362,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -892,11 +930,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O130"/>
+  <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -908,14 +946,14 @@
     <col min="5" max="5" width="28.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="34.28515625" style="1" customWidth="1"/>
     <col min="7" max="8" width="32.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="33" style="4" customWidth="1"/>
-    <col min="10" max="10" width="57.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="15" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="28.7109375" style="1" hidden="1"/>
+    <col min="9" max="10" width="33" style="4" customWidth="1"/>
+    <col min="11" max="11" width="57.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="16" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="16384" width="28.7109375" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -944,10 +982,13 @@
         <v>3</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -955,8 +996,11 @@
         <v>12</v>
       </c>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="J2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -964,8 +1008,11 @@
         <v>11</v>
       </c>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="J3" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -973,8 +1020,11 @@
         <v>13</v>
       </c>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="J4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -988,8 +1038,11 @@
         <v>17</v>
       </c>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="J5" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -997,8 +1050,11 @@
         <v>18</v>
       </c>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="J6" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1006,8 +1062,11 @@
         <v>25</v>
       </c>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+      <c r="J7" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1027,8 +1086,11 @@
         <v>24</v>
       </c>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J8" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1038,8 +1100,11 @@
       <c r="I9" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="J9" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1047,8 +1112,9 @@
         <v>29</v>
       </c>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1056,8 +1122,9 @@
         <v>30</v>
       </c>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1065,8 +1132,11 @@
         <v>31</v>
       </c>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="J12" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1074,8 +1144,11 @@
         <v>32</v>
       </c>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J13" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1085,8 +1158,11 @@
       <c r="I14" s="6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="J14" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1103,8 +1179,11 @@
         <v>35</v>
       </c>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="J15" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1121,8 +1200,11 @@
         <v>39</v>
       </c>
       <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="J16" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1130,8 +1212,11 @@
         <v>41</v>
       </c>
       <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="J17" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1139,8 +1224,11 @@
         <v>40</v>
       </c>
       <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="J18" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1157,8 +1245,11 @@
         <v>45</v>
       </c>
       <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="J19" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1175,8 +1266,11 @@
         <v>47</v>
       </c>
       <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="J20" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1184,8 +1278,11 @@
         <v>48</v>
       </c>
       <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="J21" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1193,8 +1290,11 @@
         <v>49</v>
       </c>
       <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="J22" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1211,8 +1311,11 @@
         <v>52</v>
       </c>
       <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="J23" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
@@ -1220,8 +1323,11 @@
         <v>64</v>
       </c>
       <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+      <c r="J24" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="90" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -1229,8 +1335,11 @@
         <v>53</v>
       </c>
       <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="J25" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1247,8 +1356,11 @@
         <v>56</v>
       </c>
       <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="J26" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1256,8 +1368,11 @@
         <v>57</v>
       </c>
       <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="J27" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1274,8 +1389,11 @@
         <v>60</v>
       </c>
       <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="J28" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -1292,8 +1410,11 @@
         <v>63</v>
       </c>
       <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="J29" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -1301,309 +1422,410 @@
         <v>65</v>
       </c>
       <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I55" s="1"/>
-    </row>
-    <row r="56" spans="9:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="9:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I56" s="1"/>
-    </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I57" s="1"/>
-    </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I58" s="1"/>
-    </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I59" s="1"/>
-    </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I60" s="1"/>
-    </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I62" s="1"/>
-    </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I63" s="1"/>
-    </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I64" s="1"/>
-    </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I65" s="1"/>
-    </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I66" s="1"/>
-    </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I67" s="1"/>
-    </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I68" s="1"/>
-    </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I69" s="1"/>
-    </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I70" s="1"/>
-    </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I71" s="1"/>
-    </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I72" s="1"/>
-    </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I73" s="1"/>
-    </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I74" s="1"/>
-    </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I75" s="1"/>
-    </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I76" s="1"/>
-    </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I77" s="1"/>
-    </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I78" s="1"/>
-    </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I79" s="1"/>
-    </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I80" s="1"/>
-    </row>
-    <row r="81" spans="9:9" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" spans="9:10" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I81" s="1"/>
-    </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J81" s="1"/>
+    </row>
+    <row r="82" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I82" s="1"/>
-    </row>
-    <row r="83" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J82" s="1"/>
+    </row>
+    <row r="83" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I83" s="1"/>
-    </row>
-    <row r="84" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I84" s="1"/>
-    </row>
-    <row r="85" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J84" s="1"/>
+    </row>
+    <row r="85" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I85" s="1"/>
-    </row>
-    <row r="86" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J85" s="1"/>
+    </row>
+    <row r="86" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I86" s="1"/>
-    </row>
-    <row r="87" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I87" s="1"/>
-    </row>
-    <row r="88" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J87" s="1"/>
+    </row>
+    <row r="88" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I88" s="1"/>
-    </row>
-    <row r="89" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J88" s="1"/>
+    </row>
+    <row r="89" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I89" s="1"/>
-    </row>
-    <row r="90" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J89" s="1"/>
+    </row>
+    <row r="90" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I90" s="1"/>
-    </row>
-    <row r="91" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J90" s="1"/>
+    </row>
+    <row r="91" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I91" s="1"/>
-    </row>
-    <row r="92" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J91" s="1"/>
+    </row>
+    <row r="92" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I92" s="1"/>
-    </row>
-    <row r="93" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J92" s="1"/>
+    </row>
+    <row r="93" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I93" s="1"/>
-    </row>
-    <row r="94" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J93" s="1"/>
+    </row>
+    <row r="94" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I94" s="3"/>
-    </row>
-    <row r="95" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J94" s="3"/>
+    </row>
+    <row r="95" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I95" s="1"/>
-    </row>
-    <row r="96" spans="9:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J95" s="1"/>
+    </row>
+    <row r="96" spans="9:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I96" s="1"/>
-    </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J96" s="1"/>
+    </row>
+    <row r="97" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I97" s="1"/>
-    </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J97" s="1"/>
+    </row>
+    <row r="98" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I98" s="1"/>
-    </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J98" s="1"/>
+    </row>
+    <row r="99" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I99" s="1"/>
-    </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J99" s="1"/>
+    </row>
+    <row r="100" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I100" s="1"/>
-    </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J100" s="1"/>
+    </row>
+    <row r="101" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I101" s="1"/>
-    </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J101" s="1"/>
+    </row>
+    <row r="102" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I102" s="1"/>
-    </row>
-    <row r="103" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J102" s="1"/>
+    </row>
+    <row r="103" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I103" s="1"/>
-    </row>
-    <row r="104" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J103" s="1"/>
+    </row>
+    <row r="104" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I104" s="1"/>
-    </row>
-    <row r="105" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J104" s="1"/>
+    </row>
+    <row r="105" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I105" s="1"/>
-    </row>
-    <row r="106" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J105" s="1"/>
+    </row>
+    <row r="106" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I106" s="1"/>
-    </row>
-    <row r="107" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J106" s="1"/>
+    </row>
+    <row r="107" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I107" s="1"/>
-    </row>
-    <row r="108" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J107" s="1"/>
+    </row>
+    <row r="108" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I108" s="1"/>
-    </row>
-    <row r="109" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J108" s="1"/>
+    </row>
+    <row r="109" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I109" s="1"/>
-    </row>
-    <row r="110" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J109" s="1"/>
+    </row>
+    <row r="110" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I110" s="1"/>
-    </row>
-    <row r="111" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J110" s="1"/>
+    </row>
+    <row r="111" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I111" s="1"/>
-    </row>
-    <row r="112" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J111" s="1"/>
+    </row>
+    <row r="112" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I112" s="1"/>
-    </row>
-    <row r="113" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J112" s="1"/>
+    </row>
+    <row r="113" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I113" s="1"/>
-    </row>
-    <row r="114" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J113" s="1"/>
+    </row>
+    <row r="114" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I114" s="1"/>
-    </row>
-    <row r="115" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J114" s="1"/>
+    </row>
+    <row r="115" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I115" s="1"/>
-    </row>
-    <row r="116" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J115" s="1"/>
+    </row>
+    <row r="116" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I116" s="1"/>
-    </row>
-    <row r="117" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J116" s="1"/>
+    </row>
+    <row r="117" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I117" s="1"/>
-    </row>
-    <row r="118" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J117" s="1"/>
+    </row>
+    <row r="118" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I118" s="1"/>
-    </row>
-    <row r="119" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J118" s="1"/>
+    </row>
+    <row r="119" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I119" s="1"/>
-    </row>
-    <row r="120" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J119" s="1"/>
+    </row>
+    <row r="120" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I120" s="1"/>
-    </row>
-    <row r="121" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J120" s="1"/>
+    </row>
+    <row r="121" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I121" s="1"/>
-    </row>
-    <row r="122" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J121" s="1"/>
+    </row>
+    <row r="122" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I122" s="1"/>
-    </row>
-    <row r="123" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J122" s="1"/>
+    </row>
+    <row r="123" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I123" s="1"/>
-    </row>
-    <row r="124" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J123" s="1"/>
+    </row>
+    <row r="124" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I124" s="1"/>
-    </row>
-    <row r="125" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J124" s="1"/>
+    </row>
+    <row r="125" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I125" s="1"/>
-    </row>
-    <row r="126" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J125" s="1"/>
+    </row>
+    <row r="126" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I126" s="1"/>
-    </row>
-    <row r="127" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J126" s="1"/>
+    </row>
+    <row r="127" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I127" s="1"/>
-    </row>
-    <row r="128" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J127" s="1"/>
+    </row>
+    <row r="128" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I128" s="1"/>
-    </row>
-    <row r="129" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J128" s="1"/>
+    </row>
+    <row r="129" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I129" s="1"/>
-    </row>
-    <row r="130" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J129" s="1"/>
+    </row>
+    <row r="130" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I130" s="1"/>
+      <c r="J130" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:I1 A2:A3 C2:I3 A4:I5 A12:I12 A6:A7 C6:I7 A15:I15 A13:A14 C13:I14 A17:I19 A16 C16:I16 A20 C20:I20 C9:I11 A9:A11 A21:I1048576">
+  <conditionalFormatting sqref="A1:J1 A2:A3 C2:J3 A4:J5 A12:J12 A6:A7 C6:J7 A15:J15 A13:A14 C13:J14 A17:J19 A16 C16:J16 A20 C20:J20 C9:J11 A9:A11 A21:J1048576">
     <cfRule type="expression" dxfId="39" priority="41">
       <formula>EXACT($A1,"text")</formula>
     </cfRule>
@@ -1715,7 +1937,7 @@
       <formula>EXACT($A20,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8 C8:I8">
+  <conditionalFormatting sqref="A8 C8:J8">
     <cfRule type="expression" dxfId="7" priority="5">
       <formula>EXACT($A8,"text")</formula>
     </cfRule>

</xml_diff>

<commit_message>
answer choices and correct answers separated by semicolon now
</commit_message>
<xml_diff>
--- a/inst/Data_Analysis_Modules/Module1.xlsx
+++ b/inst/Data_Analysis_Modules/Module1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
   <si>
     <t>Choices</t>
   </si>
@@ -87,10 +87,6 @@
     <t>multiple</t>
   </si>
   <si>
-    <t>Men living at the retirement home
-College students</t>
-  </si>
-  <si>
     <t>College students</t>
   </si>
   <si>
@@ -127,9 +123,6 @@
     <t>Mean, median, and mode are all measures of ____________.</t>
   </si>
   <si>
-    <t>Central tendency</t>
-  </si>
-  <si>
     <t>This is a fancy term for the "middle" of a dataset.</t>
   </si>
   <si>
@@ -251,6 +244,9 @@
   </si>
   <si>
     <t>mode</t>
+  </si>
+  <si>
+    <t>Men living at the retirement home; College students</t>
   </si>
 </sst>
 </file>
@@ -932,9 +928,9 @@
   </sheetPr>
   <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -982,7 +978,7 @@
         <v>3</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>4</v>
@@ -997,7 +993,7 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.2">
@@ -1009,7 +1005,7 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.2">
@@ -1021,7 +1017,7 @@
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.2">
@@ -1039,7 +1035,7 @@
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.2">
@@ -1051,7 +1047,7 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.2">
@@ -1059,11 +1055,11 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.2">
@@ -1071,37 +1067,37 @@
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="J9" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.2">
@@ -1109,7 +1105,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1119,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1129,11 +1125,11 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.2">
@@ -1141,25 +1137,25 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.2">
@@ -1167,20 +1163,20 @@
         <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.2">
@@ -1188,20 +1184,20 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.2">
@@ -1209,11 +1205,11 @@
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -1221,11 +1217,11 @@
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.2">
@@ -1233,20 +1229,20 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.2">
@@ -1254,20 +1250,20 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -1275,11 +1271,11 @@
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.2">
@@ -1287,11 +1283,11 @@
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.2">
@@ -1299,20 +1295,20 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.2">
@@ -1320,11 +1316,11 @@
         <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="90" x14ac:dyDescent="0.2">
@@ -1332,11 +1328,11 @@
         <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.2">
@@ -1344,20 +1340,20 @@
         <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.2">
@@ -1365,11 +1361,11 @@
         <v>10</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -1377,20 +1373,20 @@
         <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -1398,28 +1394,28 @@
         <v>19</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E29" s="1">
         <v>19</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>

</xml_diff>

<commit_message>
tags in real time and introduces additional questions if user is struggling
</commit_message>
<xml_diff>
--- a/inst/Data_Analysis_Modules/Module1.xlsx
+++ b/inst/Data_Analysis_Modules/Module1.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Dropbox\R_Working_Directory\My_Packages\swirl\inst\Data_Analysis_Modules\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22810"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23680" windowHeight="12980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A:$K</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A:$L</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="99">
   <si>
     <t>Choices</t>
   </si>
@@ -156,21 +156,12 @@
     <t>Use 'dataset$variable' notation. Remember the name of our dataset is 'cars' and the name of the variable we are interested in is 'mpgCity'.</t>
   </si>
   <si>
-    <t>Now store the contents of this variable in a new variable called 'myMPG'.</t>
-  </si>
-  <si>
-    <t>You'll have to retype your answer to the previous question, but this time use the assignment operator to assign its value to a new variable called 'myMPG'.</t>
-  </si>
-  <si>
     <t>The ARITHMETIC MEAN, or simply the MEAN or AVERAGE, is the most common measurement of central tendency. To calculate the mean of a dataset, you first sum all of the values and then divide that sum by the total number of values in the dataset.</t>
   </si>
   <si>
     <t>However, when there are many values of interest, it becomes tedious to do this calculation by hand. Luckily R has a built-in function for computing the mean. The syntax for doing so is 'mean(variable)'.</t>
   </si>
   <si>
-    <t>Compute the mean value for 'myMPG' variable now.</t>
-  </si>
-  <si>
     <t>mean(myMPG)</t>
   </si>
   <si>
@@ -201,9 +192,6 @@
     <t>Type 'table' followed by your variable name placed in parentheses. As usual, leave out the spaces.</t>
   </si>
   <si>
-    <t>The first row gives you the value of your variable and the second row gives you the number of times it appears in your dataset. Since the mode is the value of our variable that appears most frequently, what is the mode of our 'myMPG' variable?</t>
-  </si>
-  <si>
     <t>exact</t>
   </si>
   <si>
@@ -231,9 +219,6 @@
     <t>central tendency</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>sample vs. population</t>
   </si>
   <si>
@@ -247,13 +232,100 @@
   </si>
   <si>
     <t>Men living at the retirement home; College students</t>
+  </si>
+  <si>
+    <t>Let's try another example to make sure you fully understand the idea of a representative sample. If you were interested in studying a group of African animals and how they adapt to climate change, which sample would be more representative of the target population: a sample consisting of 25 lions and 25 cheetahs, or a sample consisting of 25 kangaroos and 25 koala bears?</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>25 lions and 25 cheetahs</t>
+  </si>
+  <si>
+    <t>mandatory</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>25 lions and 25 cheetahs; 25 kangaroos and 25 koala bears</t>
+  </si>
+  <si>
+    <t>Since your target population is all African animals, which of these 2 sample populations more closely matches the population of interest?</t>
+  </si>
+  <si>
+    <t>Which of the following terms are of most importance when describing the central tendency of a data set?</t>
+  </si>
+  <si>
+    <t>median, mode, range; statistics, population, mode; population, sample, representative; mode, median, mean</t>
+  </si>
+  <si>
+    <t>mode, median, mean</t>
+  </si>
+  <si>
+    <t>These are the three different methods  stated above that are used for describing the center of a data set.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Now try accessing the 'driveTrain' variable from the 'cars' dataset using the 'dataset$variable' notation. </t>
+  </si>
+  <si>
+    <t>cars$driveTrain</t>
+  </si>
+  <si>
+    <t>Use 'dataset$variable' notation. Remember the name of our dataset is 'cars' and the name of the variable we are interested in is 'driveTrain'.</t>
+  </si>
+  <si>
+    <t>Now store the contents of the 'cars$mpgCity' in a new variable called 'myMPG'.</t>
+  </si>
+  <si>
+    <t>Further, store the contents of the 'cars$driveTrain' in a new variable called 'myDrive'.</t>
+  </si>
+  <si>
+    <t>myDrive &lt;- cars$driveTrain</t>
+  </si>
+  <si>
+    <t>Use the assignment operator to assign 'cars$mpgCity' to a new variable called 'myMPG'.</t>
+  </si>
+  <si>
+    <t>Use the assignment operator to assign 'cars$driveTrain' to a new variable called 'myDrive'.</t>
+  </si>
+  <si>
+    <t>Compute the mean value for the 'myMPG' variable now.</t>
+  </si>
+  <si>
+    <t>Also, try to compute the mean value for the 'myDrive' variable now.</t>
+  </si>
+  <si>
+    <t>mean(myDrive)</t>
+  </si>
+  <si>
+    <t>Second, find the median value of your 'myDrive' variable now.</t>
+  </si>
+  <si>
+    <t>median(myDrive)</t>
+  </si>
+  <si>
+    <t>Now, try using the 'table' function on your 'myDrive' variable.</t>
+  </si>
+  <si>
+    <t>table(myDrive)</t>
+  </si>
+  <si>
+    <t>Look at your table for the 'myMPG' variable that you created above. The first row gives you the value of your variable and the second row gives you the number of times it appears in your dataset. Since the mode is the value of our variable that appears most frequently, what is the mode of your 'myMPG' variable?</t>
+  </si>
+  <si>
+    <t>This time look at your table for your 'myDrive' variable. What is the mode of your 'myDrive' variable?</t>
+  </si>
+  <si>
+    <t>R-command</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -278,8 +350,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,8 +376,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -309,36 +399,55 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -361,12 +470,80 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="8">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="48">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -703,7 +880,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -738,7 +915,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -915,7 +1092,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -923,33 +1100,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P130"/>
+  <dimension ref="A1:Q138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="75.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="32.5703125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="33" style="4" customWidth="1"/>
-    <col min="11" max="11" width="57.140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="28.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="16" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="16384" width="28.7109375" style="1" hidden="1"/>
+    <col min="1" max="1" width="20.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="75.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="34.33203125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="32.5" style="1" customWidth="1"/>
+    <col min="10" max="11" width="33" style="4" customWidth="1"/>
+    <col min="12" max="12" width="57.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="17" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="16384" width="28.6640625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="26.25" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -957,112 +1135,115 @@
         <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="K1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="30">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="30">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="45">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="45">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.2">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="60">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.2">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="75">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1070,870 +1251,1085 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="E8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="75">
+      <c r="A9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+      <c r="K10" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" s="1"/>
+        <v>28</v>
+      </c>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" ht="30">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" ht="45">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="45">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="J14" s="1"/>
+      <c r="K14" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="6" t="s">
+      <c r="B15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:13" ht="30">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="75">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="45">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="J18" s="1"/>
+      <c r="K18" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="75">
+      <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="J19" s="1"/>
+      <c r="K19" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30">
+      <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="J20" s="1"/>
+      <c r="K20" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="60">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="J21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="60">
+      <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="45">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="45">
+      <c r="A24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+      <c r="D24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="60">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="45">
       <c r="A26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="60">
+      <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="F27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="60">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="60">
+      <c r="A29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="1">
-        <v>19</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="J29" s="1"/>
+      <c r="K29" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="90">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30" s="1"/>
+        <v>48</v>
+      </c>
       <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I31" s="1"/>
+      <c r="K30" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="60">
+      <c r="A31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I32" s="1"/>
+      <c r="K31" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="60">
+      <c r="A32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I33" s="1"/>
+      <c r="K32" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="60">
+      <c r="A33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I34" s="1"/>
+      <c r="K33" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="45">
+      <c r="A34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I35" s="1"/>
+      <c r="K34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="45">
+      <c r="A35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I36" s="1"/>
+      <c r="K35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="60">
+      <c r="A36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="1">
+        <v>19</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I37" s="1"/>
+      <c r="K36" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="60">
+      <c r="A37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="1">
+        <v>43</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I38" s="1"/>
+      <c r="K37" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="60">
+      <c r="A38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I39" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="1:11">
       <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I40" s="1"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:11">
       <c r="J40" s="1"/>
-    </row>
-    <row r="41" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I41" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:11">
       <c r="J41" s="1"/>
-    </row>
-    <row r="42" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I42" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11">
       <c r="J42" s="1"/>
-    </row>
-    <row r="43" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I43" s="1"/>
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11">
       <c r="J43" s="1"/>
-    </row>
-    <row r="44" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I44" s="1"/>
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="1:11">
       <c r="J44" s="1"/>
-    </row>
-    <row r="45" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I45" s="1"/>
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="1:11">
       <c r="J45" s="1"/>
-    </row>
-    <row r="46" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I46" s="1"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11">
       <c r="J46" s="1"/>
-    </row>
-    <row r="47" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I47" s="1"/>
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:11">
       <c r="J47" s="1"/>
-    </row>
-    <row r="48" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I48" s="1"/>
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="1:11">
       <c r="J48" s="1"/>
-    </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I49" s="1"/>
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="10:11">
       <c r="J49" s="1"/>
-    </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I50" s="1"/>
+      <c r="K49" s="1"/>
+    </row>
+    <row r="50" spans="10:11">
       <c r="J50" s="1"/>
-    </row>
-    <row r="51" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I51" s="1"/>
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="10:11">
       <c r="J51" s="1"/>
-    </row>
-    <row r="52" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I52" s="1"/>
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="10:11">
       <c r="J52" s="1"/>
-    </row>
-    <row r="53" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I53" s="1"/>
+      <c r="K52" s="1"/>
+    </row>
+    <row r="53" spans="10:11">
       <c r="J53" s="1"/>
-    </row>
-    <row r="54" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I54" s="1"/>
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="10:11">
       <c r="J54" s="1"/>
-    </row>
-    <row r="55" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I55" s="1"/>
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="10:11">
       <c r="J55" s="1"/>
-    </row>
-    <row r="56" spans="9:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I56" s="1"/>
+      <c r="K55" s="1"/>
+    </row>
+    <row r="56" spans="10:11">
       <c r="J56" s="1"/>
-    </row>
-    <row r="57" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I57" s="1"/>
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="10:11">
       <c r="J57" s="1"/>
-    </row>
-    <row r="58" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I58" s="1"/>
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="10:11">
       <c r="J58" s="1"/>
-    </row>
-    <row r="59" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I59" s="1"/>
+      <c r="K58" s="1"/>
+    </row>
+    <row r="59" spans="10:11">
       <c r="J59" s="1"/>
-    </row>
-    <row r="60" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I60" s="1"/>
+      <c r="K59" s="1"/>
+    </row>
+    <row r="60" spans="10:11">
       <c r="J60" s="1"/>
-    </row>
-    <row r="61" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I61" s="1"/>
+      <c r="K60" s="1"/>
+    </row>
+    <row r="61" spans="10:11">
       <c r="J61" s="1"/>
-    </row>
-    <row r="62" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I62" s="1"/>
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" spans="10:11">
       <c r="J62" s="1"/>
-    </row>
-    <row r="63" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I63" s="1"/>
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="10:11">
       <c r="J63" s="1"/>
-    </row>
-    <row r="64" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I64" s="1"/>
+      <c r="K63" s="1"/>
+    </row>
+    <row r="64" spans="10:11" ht="55.5" customHeight="1">
       <c r="J64" s="1"/>
-    </row>
-    <row r="65" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I65" s="1"/>
+      <c r="K64" s="1"/>
+    </row>
+    <row r="65" spans="10:11">
       <c r="J65" s="1"/>
-    </row>
-    <row r="66" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I66" s="1"/>
+      <c r="K65" s="1"/>
+    </row>
+    <row r="66" spans="10:11">
       <c r="J66" s="1"/>
-    </row>
-    <row r="67" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I67" s="1"/>
+      <c r="K66" s="1"/>
+    </row>
+    <row r="67" spans="10:11">
       <c r="J67" s="1"/>
-    </row>
-    <row r="68" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I68" s="1"/>
+      <c r="K67" s="1"/>
+    </row>
+    <row r="68" spans="10:11">
       <c r="J68" s="1"/>
-    </row>
-    <row r="69" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I69" s="1"/>
+      <c r="K68" s="1"/>
+    </row>
+    <row r="69" spans="10:11">
       <c r="J69" s="1"/>
-    </row>
-    <row r="70" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I70" s="1"/>
+      <c r="K69" s="1"/>
+    </row>
+    <row r="70" spans="10:11">
       <c r="J70" s="1"/>
-    </row>
-    <row r="71" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I71" s="1"/>
+      <c r="K70" s="1"/>
+    </row>
+    <row r="71" spans="10:11">
       <c r="J71" s="1"/>
-    </row>
-    <row r="72" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I72" s="1"/>
+      <c r="K71" s="1"/>
+    </row>
+    <row r="72" spans="10:11">
       <c r="J72" s="1"/>
-    </row>
-    <row r="73" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I73" s="1"/>
+      <c r="K72" s="1"/>
+    </row>
+    <row r="73" spans="10:11">
       <c r="J73" s="1"/>
-    </row>
-    <row r="74" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I74" s="1"/>
+      <c r="K73" s="1"/>
+    </row>
+    <row r="74" spans="10:11">
       <c r="J74" s="1"/>
-    </row>
-    <row r="75" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I75" s="1"/>
+      <c r="K74" s="1"/>
+    </row>
+    <row r="75" spans="10:11">
       <c r="J75" s="1"/>
-    </row>
-    <row r="76" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I76" s="1"/>
+      <c r="K75" s="1"/>
+    </row>
+    <row r="76" spans="10:11">
       <c r="J76" s="1"/>
-    </row>
-    <row r="77" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I77" s="1"/>
+      <c r="K76" s="1"/>
+    </row>
+    <row r="77" spans="10:11">
       <c r="J77" s="1"/>
-    </row>
-    <row r="78" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I78" s="1"/>
+      <c r="K77" s="1"/>
+    </row>
+    <row r="78" spans="10:11">
       <c r="J78" s="1"/>
-    </row>
-    <row r="79" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I79" s="1"/>
+      <c r="K78" s="1"/>
+    </row>
+    <row r="79" spans="10:11">
       <c r="J79" s="1"/>
-    </row>
-    <row r="80" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I80" s="1"/>
+      <c r="K79" s="1"/>
+    </row>
+    <row r="80" spans="10:11">
       <c r="J80" s="1"/>
-    </row>
-    <row r="81" spans="9:10" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I81" s="1"/>
+      <c r="K80" s="1"/>
+    </row>
+    <row r="81" spans="10:11">
       <c r="J81" s="1"/>
-    </row>
-    <row r="82" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I82" s="1"/>
+      <c r="K81" s="1"/>
+    </row>
+    <row r="82" spans="10:11">
       <c r="J82" s="1"/>
-    </row>
-    <row r="83" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I83" s="1"/>
+      <c r="K82" s="1"/>
+    </row>
+    <row r="83" spans="10:11">
       <c r="J83" s="1"/>
-    </row>
-    <row r="84" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I84" s="1"/>
+      <c r="K83" s="1"/>
+    </row>
+    <row r="84" spans="10:11">
       <c r="J84" s="1"/>
-    </row>
-    <row r="85" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I85" s="1"/>
+      <c r="K84" s="1"/>
+    </row>
+    <row r="85" spans="10:11">
       <c r="J85" s="1"/>
-    </row>
-    <row r="86" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I86" s="1"/>
+      <c r="K85" s="1"/>
+    </row>
+    <row r="86" spans="10:11">
       <c r="J86" s="1"/>
-    </row>
-    <row r="87" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I87" s="1"/>
+      <c r="K86" s="1"/>
+    </row>
+    <row r="87" spans="10:11">
       <c r="J87" s="1"/>
-    </row>
-    <row r="88" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I88" s="1"/>
+      <c r="K87" s="1"/>
+    </row>
+    <row r="88" spans="10:11">
       <c r="J88" s="1"/>
-    </row>
-    <row r="89" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I89" s="1"/>
+      <c r="K88" s="1"/>
+    </row>
+    <row r="89" spans="10:11" ht="133.5" customHeight="1">
       <c r="J89" s="1"/>
-    </row>
-    <row r="90" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I90" s="1"/>
+      <c r="K89" s="1"/>
+    </row>
+    <row r="90" spans="10:11">
       <c r="J90" s="1"/>
-    </row>
-    <row r="91" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I91" s="1"/>
+      <c r="K90" s="1"/>
+    </row>
+    <row r="91" spans="10:11">
       <c r="J91" s="1"/>
-    </row>
-    <row r="92" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I92" s="1"/>
+      <c r="K91" s="1"/>
+    </row>
+    <row r="92" spans="10:11">
       <c r="J92" s="1"/>
-    </row>
-    <row r="93" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I93" s="1"/>
+      <c r="K92" s="1"/>
+    </row>
+    <row r="93" spans="10:11">
       <c r="J93" s="1"/>
-    </row>
-    <row r="94" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I94" s="3"/>
-      <c r="J94" s="3"/>
-    </row>
-    <row r="95" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I95" s="1"/>
+      <c r="K93" s="1"/>
+    </row>
+    <row r="94" spans="10:11">
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+    </row>
+    <row r="95" spans="10:11">
       <c r="J95" s="1"/>
-    </row>
-    <row r="96" spans="9:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I96" s="1"/>
+      <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="10:11">
       <c r="J96" s="1"/>
-    </row>
-    <row r="97" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I97" s="1"/>
+      <c r="K96" s="1"/>
+    </row>
+    <row r="97" spans="10:11">
       <c r="J97" s="1"/>
-    </row>
-    <row r="98" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I98" s="1"/>
+      <c r="K97" s="1"/>
+    </row>
+    <row r="98" spans="10:11">
       <c r="J98" s="1"/>
-    </row>
-    <row r="99" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I99" s="1"/>
+      <c r="K98" s="1"/>
+    </row>
+    <row r="99" spans="10:11">
       <c r="J99" s="1"/>
-    </row>
-    <row r="100" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I100" s="1"/>
+      <c r="K99" s="1"/>
+    </row>
+    <row r="100" spans="10:11">
       <c r="J100" s="1"/>
-    </row>
-    <row r="101" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I101" s="1"/>
+      <c r="K100" s="1"/>
+    </row>
+    <row r="101" spans="10:11">
       <c r="J101" s="1"/>
-    </row>
-    <row r="102" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
-    </row>
-    <row r="103" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I103" s="1"/>
+      <c r="K101" s="1"/>
+    </row>
+    <row r="102" spans="10:11">
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+    </row>
+    <row r="103" spans="10:11">
       <c r="J103" s="1"/>
-    </row>
-    <row r="104" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I104" s="1"/>
+      <c r="K103" s="1"/>
+    </row>
+    <row r="104" spans="10:11" ht="52.5" customHeight="1">
       <c r="J104" s="1"/>
-    </row>
-    <row r="105" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I105" s="1"/>
+      <c r="K104" s="1"/>
+    </row>
+    <row r="105" spans="10:11">
       <c r="J105" s="1"/>
-    </row>
-    <row r="106" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I106" s="1"/>
+      <c r="K105" s="1"/>
+    </row>
+    <row r="106" spans="10:11">
       <c r="J106" s="1"/>
-    </row>
-    <row r="107" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I107" s="1"/>
+      <c r="K106" s="1"/>
+    </row>
+    <row r="107" spans="10:11">
       <c r="J107" s="1"/>
-    </row>
-    <row r="108" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I108" s="1"/>
+      <c r="K107" s="1"/>
+    </row>
+    <row r="108" spans="10:11">
       <c r="J108" s="1"/>
-    </row>
-    <row r="109" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I109" s="1"/>
+      <c r="K108" s="1"/>
+    </row>
+    <row r="109" spans="10:11">
       <c r="J109" s="1"/>
-    </row>
-    <row r="110" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I110" s="1"/>
+      <c r="K109" s="1"/>
+    </row>
+    <row r="110" spans="10:11">
       <c r="J110" s="1"/>
-    </row>
-    <row r="111" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I111" s="1"/>
+      <c r="K110" s="1"/>
+    </row>
+    <row r="111" spans="10:11">
       <c r="J111" s="1"/>
-    </row>
-    <row r="112" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I112" s="1"/>
+      <c r="K111" s="1"/>
+    </row>
+    <row r="112" spans="10:11">
       <c r="J112" s="1"/>
-    </row>
-    <row r="113" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I113" s="1"/>
+      <c r="K112" s="1"/>
+    </row>
+    <row r="113" spans="10:11">
       <c r="J113" s="1"/>
-    </row>
-    <row r="114" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I114" s="1"/>
+      <c r="K113" s="1"/>
+    </row>
+    <row r="114" spans="10:11">
       <c r="J114" s="1"/>
-    </row>
-    <row r="115" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I115" s="1"/>
+      <c r="K114" s="1"/>
+    </row>
+    <row r="115" spans="10:11">
       <c r="J115" s="1"/>
-    </row>
-    <row r="116" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I116" s="1"/>
+      <c r="K115" s="1"/>
+    </row>
+    <row r="116" spans="10:11">
       <c r="J116" s="1"/>
-    </row>
-    <row r="117" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I117" s="1"/>
+      <c r="K116" s="1"/>
+    </row>
+    <row r="117" spans="10:11">
       <c r="J117" s="1"/>
-    </row>
-    <row r="118" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I118" s="1"/>
+      <c r="K117" s="1"/>
+    </row>
+    <row r="118" spans="10:11">
       <c r="J118" s="1"/>
-    </row>
-    <row r="119" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I119" s="1"/>
+      <c r="K118" s="1"/>
+    </row>
+    <row r="119" spans="10:11">
       <c r="J119" s="1"/>
-    </row>
-    <row r="120" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I120" s="1"/>
+      <c r="K119" s="1"/>
+    </row>
+    <row r="120" spans="10:11">
       <c r="J120" s="1"/>
-    </row>
-    <row r="121" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I121" s="1"/>
+      <c r="K120" s="1"/>
+    </row>
+    <row r="121" spans="10:11">
       <c r="J121" s="1"/>
-    </row>
-    <row r="122" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I122" s="1"/>
+      <c r="K121" s="1"/>
+    </row>
+    <row r="122" spans="10:11">
       <c r="J122" s="1"/>
-    </row>
-    <row r="123" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I123" s="1"/>
+      <c r="K122" s="1"/>
+    </row>
+    <row r="123" spans="10:11">
       <c r="J123" s="1"/>
-    </row>
-    <row r="124" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I124" s="1"/>
+      <c r="K123" s="1"/>
+    </row>
+    <row r="124" spans="10:11">
       <c r="J124" s="1"/>
-    </row>
-    <row r="125" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I125" s="1"/>
+      <c r="K124" s="1"/>
+    </row>
+    <row r="125" spans="10:11">
       <c r="J125" s="1"/>
-    </row>
-    <row r="126" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I126" s="1"/>
+      <c r="K125" s="1"/>
+    </row>
+    <row r="126" spans="10:11">
       <c r="J126" s="1"/>
-    </row>
-    <row r="127" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I127" s="1"/>
+      <c r="K126" s="1"/>
+    </row>
+    <row r="127" spans="10:11">
       <c r="J127" s="1"/>
-    </row>
-    <row r="128" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I128" s="1"/>
+      <c r="K127" s="1"/>
+    </row>
+    <row r="128" spans="10:11">
       <c r="J128" s="1"/>
-    </row>
-    <row r="129" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I129" s="1"/>
+      <c r="K128" s="1"/>
+    </row>
+    <row r="129" spans="10:11">
       <c r="J129" s="1"/>
-    </row>
-    <row r="130" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I130" s="1"/>
+      <c r="K129" s="1"/>
+    </row>
+    <row r="130" spans="10:11">
       <c r="J130" s="1"/>
+      <c r="K130" s="1"/>
+    </row>
+    <row r="131" spans="10:11">
+      <c r="J131" s="1"/>
+      <c r="K131" s="1"/>
+    </row>
+    <row r="132" spans="10:11">
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+    </row>
+    <row r="133" spans="10:11">
+      <c r="J133" s="1"/>
+      <c r="K133" s="1"/>
+    </row>
+    <row r="134" spans="10:11">
+      <c r="J134" s="1"/>
+      <c r="K134" s="1"/>
+    </row>
+    <row r="135" spans="10:11">
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+    </row>
+    <row r="136" spans="10:11">
+      <c r="J136" s="1"/>
+      <c r="K136" s="1"/>
+    </row>
+    <row r="137" spans="10:11">
+      <c r="J137" s="1"/>
+      <c r="K137" s="1"/>
+    </row>
+    <row r="138" spans="10:11">
+      <c r="J138" s="1"/>
+      <c r="K138" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:J1 A2:A3 C2:J3 A4:J5 A12:J12 A6:A7 C6:J7 A15:J15 A13:A14 C13:J14 A17:J19 A16 C16:J16 A20 C20:J20 C9:J11 A9:A11 A21:J1048576">
-    <cfRule type="expression" dxfId="39" priority="41">
+  <conditionalFormatting sqref="A1:K1 A2:A3 D2:K3 A4:K5 A13:K13 A6:A7 D6:K7 A14:A15 D14:K15 A23:A24 D10:K12 A10:A12 A16:K22 D23:K24 A25:K1048576">
+    <cfRule type="expression" dxfId="35" priority="41">
       <formula>EXACT($A1,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="46">
+    <cfRule type="expression" dxfId="34" priority="46">
       <formula>EXACT($A1,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="47">
+    <cfRule type="expression" dxfId="33" priority="47">
       <formula>EXACT($A1,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="48">
+    <cfRule type="expression" dxfId="32" priority="48">
       <formula>EXACT($A1,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="expression" dxfId="35" priority="37">
+  <conditionalFormatting sqref="B2:C3">
+    <cfRule type="expression" dxfId="31" priority="37">
       <formula>EXACT($A2,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="38">
+    <cfRule type="expression" dxfId="30" priority="38">
       <formula>EXACT($A2,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="39">
+    <cfRule type="expression" dxfId="29" priority="39">
       <formula>EXACT($A2,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="40">
+    <cfRule type="expression" dxfId="28" priority="40">
       <formula>EXACT($A2,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="31" priority="33">
+  <conditionalFormatting sqref="B6:C6">
+    <cfRule type="expression" dxfId="27" priority="33">
       <formula>EXACT($A6,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="34">
+    <cfRule type="expression" dxfId="26" priority="34">
       <formula>EXACT($A6,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="35">
+    <cfRule type="expression" dxfId="25" priority="35">
       <formula>EXACT($A6,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="36">
+    <cfRule type="expression" dxfId="24" priority="36">
       <formula>EXACT($A6,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="27" priority="25">
+  <conditionalFormatting sqref="B7:C7">
+    <cfRule type="expression" dxfId="23" priority="25">
       <formula>EXACT($A7,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="26">
+    <cfRule type="expression" dxfId="22" priority="26">
       <formula>EXACT($A7,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="27">
+    <cfRule type="expression" dxfId="21" priority="27">
       <formula>EXACT($A7,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="28">
+    <cfRule type="expression" dxfId="20" priority="28">
       <formula>EXACT($A7,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:B11">
-    <cfRule type="expression" dxfId="23" priority="21">
-      <formula>EXACT($A9,"text")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="22">
-      <formula>EXACT($A9,"video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="23">
-      <formula>EXACT($A9,"question")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="24">
-      <formula>EXACT($A9,"figure")</formula>
+  <conditionalFormatting sqref="B10:C12">
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>EXACT($A10,"text")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>EXACT($A10,"video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>EXACT($A10,"question")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>EXACT($A10,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B14">
-    <cfRule type="expression" dxfId="19" priority="17">
-      <formula>EXACT($A13,"text")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="18">
-      <formula>EXACT($A13,"video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="19">
-      <formula>EXACT($A13,"question")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20">
-      <formula>EXACT($A13,"figure")</formula>
+  <conditionalFormatting sqref="B14:C15">
+    <cfRule type="expression" dxfId="15" priority="17">
+      <formula>EXACT($A14,"text")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="18">
+      <formula>EXACT($A14,"video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="19">
+      <formula>EXACT($A14,"question")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="20">
+      <formula>EXACT($A14,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="15" priority="13">
-      <formula>EXACT($A16,"text")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="14">
-      <formula>EXACT($A16,"video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="15">
-      <formula>EXACT($A16,"question")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="16">
-      <formula>EXACT($A16,"figure")</formula>
+  <conditionalFormatting sqref="B23:C24">
+    <cfRule type="expression" dxfId="11" priority="9">
+      <formula>EXACT($A23,"text")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>EXACT($A23,"video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>EXACT($A23,"question")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="12">
+      <formula>EXACT($A23,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="11" priority="9">
-      <formula>EXACT($A20,"text")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="10">
-      <formula>EXACT($A20,"video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11">
-      <formula>EXACT($A20,"question")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12">
-      <formula>EXACT($A20,"figure")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8 C8:J8">
+  <conditionalFormatting sqref="A8 D8:K8">
     <cfRule type="expression" dxfId="7" priority="5">
       <formula>EXACT($A8,"text")</formula>
     </cfRule>
@@ -1947,7 +2343,7 @@
       <formula>EXACT($A8,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
+  <conditionalFormatting sqref="B8:C8">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>EXACT($A8,"text")</formula>
     </cfRule>
@@ -1962,6 +2358,11 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="37" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="37" fitToHeight="0" orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>